<commit_message>
SQL Script for database
</commit_message>
<xml_diff>
--- a/Table layout .xlsx
+++ b/Table layout .xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnazzaro\Documents\GitHub\talkshop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Teached Table (child) - Teacher" sheetId="1" r:id="rId4"/>
-    <sheet name="Speaker Table (child)" sheetId="2" r:id="rId5"/>
-    <sheet name="Teacher Listings" sheetId="3" r:id="rId6"/>
+    <sheet name="Teached Table (child) - Teacher" sheetId="1" r:id="rId1"/>
+    <sheet name="Speaker Table (child)" sheetId="2" r:id="rId2"/>
+    <sheet name="Teacher Listings" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>Teachers Table</t>
   </si>
@@ -92,16 +99,43 @@
   </si>
   <si>
     <t>varchar(250)</t>
+  </si>
+  <si>
+    <t>pid</t>
+  </si>
+  <si>
+    <t>School/Place of Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age group </t>
+  </si>
+  <si>
+    <t xml:space="preserve">description </t>
+  </si>
+  <si>
+    <t>int(10)</t>
+  </si>
+  <si>
+    <t>auto)Increment</t>
+  </si>
+  <si>
+    <t>Varchar(99)</t>
+  </si>
+  <si>
+    <t>Varchar(250)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contacts Email </t>
+  </si>
+  <si>
+    <t>Varch(99)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -118,7 +152,7 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -169,42 +203,45 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -215,24 +252,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -424,7 +522,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -433,7 +531,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -442,7 +540,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -451,7 +549,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -460,7 +558,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -469,7 +567,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -581,8 +679,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -590,14 +688,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -616,7 +714,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -624,7 +722,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -652,7 +750,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -678,7 +776,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -704,7 +802,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -730,7 +828,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -756,7 +854,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -782,7 +880,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -808,7 +906,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -834,7 +932,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -860,7 +958,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -873,9 +971,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -891,7 +995,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -910,7 +1014,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -936,7 +1040,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -962,7 +1066,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -988,7 +1092,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1014,7 +1118,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1040,7 +1144,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1066,7 +1170,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1092,7 +1196,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1118,7 +1222,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1144,7 +1248,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1157,9 +1261,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1172,7 +1282,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1191,7 +1301,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1221,7 +1331,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1247,7 +1357,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1273,7 +1383,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1299,7 +1409,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1325,7 +1435,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1351,7 +1461,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1377,7 +1487,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1403,7 +1513,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1429,7 +1539,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1442,346 +1552,347 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I23"/>
+  <dimension ref="A1:IV23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.05469" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.05469" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.05469" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.05469" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.05469" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.05469" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.05469" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.05469" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.05469" style="1" customWidth="1"/>
-    <col min="10" max="256" width="9.05469" style="1" customWidth="1"/>
+    <col min="1" max="256" width="9.09765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" ht="32.55" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="5">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s" s="6">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="5">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s" s="6">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="5">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s" s="6">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" t="s" s="5">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s" s="6">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" t="s" s="5">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s" s="6">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="5">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s" s="6">
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" t="s" s="5">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s" s="6">
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" t="s" s="5">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s" s="6">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" t="s" s="5">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s" s="6">
+      <c r="B12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s" s="6">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
@@ -1789,170 +1900,167 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:H12"/>
+  <dimension ref="A1:IV12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19921875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="0.25" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.25" style="7" customWidth="1"/>
-    <col min="3" max="3" width="11.25" style="7" customWidth="1"/>
-    <col min="4" max="4" width="11.25" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.25" style="7" customWidth="1"/>
-    <col min="6" max="6" width="11.25" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.25" style="7" customWidth="1"/>
-    <col min="8" max="8" width="11.25" style="7" customWidth="1"/>
-    <col min="9" max="256" width="12.25" style="7" customWidth="1"/>
+    <col min="1" max="1" width="0.19921875" style="6" customWidth="1"/>
+    <col min="2" max="8" width="11.19921875" style="6" customWidth="1"/>
+    <col min="9" max="256" width="12.19921875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="2" customHeight="1"/>
-    <row r="2" ht="35.1" customHeight="1">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" ht="35.1" customHeight="1">
-      <c r="B3" t="s" s="5">
+    <row r="1" spans="2:8" ht="2.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" ht="34.75" customHeight="1">
-      <c r="B4" t="s" s="5">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="2:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s" s="6">
+      <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" ht="34.75" customHeight="1">
-      <c r="B5" t="s" s="5">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="2:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s" s="6">
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" ht="34.75" customHeight="1">
-      <c r="B6" t="s" s="5">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="2:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s" s="6">
+      <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" ht="34.75" customHeight="1">
-      <c r="B7" t="s" s="5">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="2:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s" s="6">
+      <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" ht="34.75" customHeight="1">
-      <c r="B8" t="s" s="5">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="2:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s" s="6">
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" ht="34.75" customHeight="1">
-      <c r="B9" t="s" s="5">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="2:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s" s="6">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" ht="34.75" customHeight="1">
-      <c r="B10" t="s" s="5">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s" s="6">
+      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" ht="34.75" customHeight="1">
-      <c r="B11" t="s" s="5">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s" s="6">
+      <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" ht="34.75" customHeight="1">
-      <c r="B12" s="9"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="2:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
@@ -1960,136 +2068,160 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:G14"/>
+  <dimension ref="A1:IV14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19921875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="0.25" style="10" customWidth="1"/>
-    <col min="2" max="2" width="13.4297" style="10" customWidth="1"/>
-    <col min="3" max="3" width="13.4297" style="10" customWidth="1"/>
-    <col min="4" max="4" width="13.4297" style="10" customWidth="1"/>
-    <col min="5" max="5" width="13.4297" style="10" customWidth="1"/>
-    <col min="6" max="6" width="13.4297" style="10" customWidth="1"/>
-    <col min="7" max="7" width="13.4297" style="10" customWidth="1"/>
-    <col min="8" max="256" width="12.25" style="10" customWidth="1"/>
+    <col min="1" max="1" width="0.19921875" style="9" customWidth="1"/>
+    <col min="2" max="7" width="13.3984375" style="9" customWidth="1"/>
+    <col min="8" max="256" width="12.19921875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="2" customHeight="1"/>
-    <row r="2" ht="32.7" customHeight="1">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" ht="32.7" customHeight="1">
-      <c r="B3" s="9"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" ht="32.35" customHeight="1">
-      <c r="B4" s="9"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" ht="32.35" customHeight="1">
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" ht="32.35" customHeight="1">
-      <c r="B6" s="9"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" ht="32.35" customHeight="1">
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" ht="32.35" customHeight="1">
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" ht="32.35" customHeight="1">
-      <c r="B9" s="9"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" ht="32.35" customHeight="1">
-      <c r="B10" s="9"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" ht="32.35" customHeight="1">
-      <c r="B11" s="9"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" ht="32.35" customHeight="1">
-      <c r="B12" s="9"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" ht="32.35" customHeight="1">
-      <c r="B13" s="9"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" ht="32.35" customHeight="1">
-      <c r="B14" s="9"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+    <row r="1" spans="2:7" ht="2.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="2:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="2:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="8"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>